<commit_message>
Upload EmailandURLExtractor and associated files
</commit_message>
<xml_diff>
--- a/Dataset A.xlsx
+++ b/Dataset A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d40c1be7177d6ff/Documents/Programming Projects/Excel Utils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d40c1be7177d6ff/Documents/Programming Projects/Excel-Utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFC3C436-C395-4065-882C-B0FDAC90B8DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{AFC3C436-C395-4065-882C-B0FDAC90B8DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2AB08475-819C-4A46-8252-32950C697A66}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOCK_DATA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -344,12 +344,75 @@
   </si>
   <si>
     <t>Registered Nurse</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://latimes.com/donec/vitae/nisi/nam/ultrices.json?convallis=sapien&amp;morbi=iaculis&amp;odio=congue&amp;odio=vivamus&amp;elementum=metus&amp;eu=arcu&amp;interdum=adipiscing&amp;eu=molestie&amp;tincidunt=hendrerit&amp;in=at&amp;leo=vulputate&amp;maecenas=vitae&amp;pulvinar=nisl&amp;lobortis=aenean&amp;est=lectus&amp;phasellus=pellentesque&amp;sit=eget&amp;amet=nunc&amp;erat=donec&amp;nulla=quis&amp;tempus=orci</t>
+  </si>
+  <si>
+    <t>http://omniture.com/sed/vestibulum/sit.html?nisl=pulvinar&amp;aenean=nulla&amp;lectus=pede&amp;pellentesque=ullamcorper&amp;eget=augue&amp;nunc=a&amp;donec=suscipit&amp;quis=nulla&amp;orci=elit&amp;eget=ac&amp;orci=nulla&amp;vehicula=sed&amp;condimentum=vel&amp;curabitur=enim&amp;in=sit&amp;libero=amet&amp;ut=nunc&amp;massa=viverra&amp;volutpat=dapibus&amp;convallis=nulla&amp;morbi=suscipit&amp;odio=ligula&amp;odio=in&amp;elementum=lacus&amp;eu=curabitur&amp;interdum=at&amp;eu=ipsum&amp;tincidunt=ac&amp;in=tellus&amp;leo=semper&amp;maecenas=interdum&amp;pulvinar=mauris&amp;lobortis=ullamcorper</t>
+  </si>
+  <si>
+    <t>https://cam.ac.uk/purus/phasellus/in/felis.js?eget=quisque&amp;vulputate=erat&amp;ut=eros&amp;ultrices=viverra&amp;vel=eget&amp;augue=congue&amp;vestibulum=eget&amp;ante=semper&amp;ipsum=rutrum&amp;primis=nulla&amp;in=nunc&amp;faucibus=purus&amp;orci=phasellus&amp;luctus=in&amp;et=felis&amp;ultrices=donec&amp;posuere=semper&amp;cubilia=sapien&amp;curae=a&amp;donec=libero&amp;pharetra=nam&amp;magna=dui&amp;vestibulum=proin&amp;aliquet=leo&amp;ultrices=odio&amp;erat=porttitor&amp;tortor=id&amp;sollicitudin=consequat&amp;mi=in&amp;sit=consequat&amp;amet=ut&amp;lobortis=nulla&amp;sapien=sed&amp;sapien=accumsan&amp;non=felis&amp;mi=ut&amp;integer=at&amp;ac=dolor&amp;neque=quis&amp;duis=odio&amp;bibendum=consequat&amp;morbi=varius&amp;non=integer&amp;quam=ac&amp;nec=leo&amp;dui=pellentesque&amp;luctus=ultrices&amp;rutrum=mattis&amp;nulla=odio&amp;tellus=donec&amp;in=vitae&amp;sagittis=nisi&amp;dui=nam&amp;vel=ultrices&amp;nisl=libero&amp;duis=non&amp;ac=mattis&amp;nibh=pulvinar&amp;fusce=nulla&amp;lacus=pede&amp;purus=ullamcorper&amp;aliquet=augue&amp;at=a&amp;feugiat=suscipit&amp;non=nulla&amp;pretium=elit&amp;quis=ac&amp;lectus=nulla&amp;suspendisse=sed&amp;potenti=vel&amp;in=enim&amp;eleifend=sit&amp;quam=amet&amp;a=nunc&amp;odio=viverra&amp;in=dapibus&amp;hac=nulla&amp;habitasse=suscipit&amp;platea=ligula&amp;dictumst=in&amp;maecenas=lacus</t>
+  </si>
+  <si>
+    <t>https://163.com/blandit/nam/nulla/integer/pede/justo.aspx?nullam=pulvinar&amp;varius=lobortis&amp;nulla=est&amp;facilisi=phasellus&amp;cras=sit&amp;non=amet&amp;velit=erat&amp;nec=nulla&amp;nisi=tempus&amp;vulputate=vivamus&amp;nonummy=in&amp;maecenas=felis&amp;tincidunt=eu&amp;lacus=sapien&amp;at=cursus&amp;velit=vestibulum&amp;vivamus=proin&amp;vel=eu&amp;nulla=mi&amp;eget=nulla&amp;eros=ac&amp;elementum=enim&amp;pellentesque=in&amp;quisque=tempor&amp;porta=turpis&amp;volutpat=nec&amp;erat=euismod&amp;quisque=scelerisque&amp;erat=quam&amp;eros=turpis&amp;viverra=adipiscing&amp;eget=lorem&amp;congue=vitae&amp;eget=mattis&amp;semper=nibh&amp;rutrum=ligula&amp;nulla=nec&amp;nunc=sem&amp;purus=duis&amp;phasellus=aliquam&amp;in=convallis&amp;felis=nunc&amp;donec=proin&amp;semper=at&amp;sapien=turpis&amp;a=a&amp;libero=pede&amp;nam=posuere&amp;dui=nonummy&amp;proin=integer&amp;leo=non&amp;odio=velit&amp;porttitor=donec&amp;id=diam&amp;consequat=neque&amp;in=vestibulum&amp;consequat=eget&amp;ut=vulputate&amp;nulla=ut&amp;sed=ultrices&amp;accumsan=vel&amp;felis=augue&amp;ut=vestibulum&amp;at=ante&amp;dolor=ipsum&amp;quis=primis&amp;odio=in&amp;consequat=faucibus&amp;varius=orci&amp;integer=luctus&amp;ac=et&amp;leo=ultrices&amp;pellentesque=posuere&amp;ultrices=cubilia&amp;mattis=curae&amp;odio=donec&amp;donec=pharetra&amp;vitae=magna&amp;nisi=vestibulum&amp;nam=aliquet&amp;ultrices=ultrices&amp;libero=erat&amp;non=tortor&amp;mattis=sollicitudin&amp;pulvinar=mi&amp;nulla=sit</t>
+  </si>
+  <si>
+    <t>http://wiley.com/in/faucibus.html?congue=nulla&amp;vivamus=facilisi&amp;metus=cras&amp;arcu=non&amp;adipiscing=velit&amp;molestie=nec&amp;hendrerit=nisi&amp;at=vulputate&amp;vulputate=nonummy&amp;vitae=maecenas&amp;nisl=tincidunt&amp;aenean=lacus&amp;lectus=at&amp;pellentesque=velit&amp;eget=vivamus&amp;nunc=vel&amp;donec=nulla&amp;quis=eget&amp;orci=eros&amp;eget=elementum&amp;orci=pellentesque&amp;vehicula=quisque&amp;condimentum=porta&amp;curabitur=volutpat&amp;in=erat&amp;libero=quisque&amp;ut=erat&amp;massa=eros&amp;volutpat=viverra&amp;convallis=eget</t>
+  </si>
+  <si>
+    <t>http://booking.com/aenean/lectus/pellentesque/eget/nunc/donec.xml?mauris=fermentum&amp;enim=justo&amp;leo=nec&amp;rhoncus=condimentum&amp;sed=neque&amp;vestibulum=sapien&amp;sit=placerat&amp;amet=ante&amp;cursus=nulla&amp;id=justo&amp;turpis=aliquam&amp;integer=quis&amp;aliquet=turpis&amp;massa=eget&amp;id=elit&amp;lobortis=sodales&amp;convallis=scelerisque&amp;tortor=mauris&amp;risus=sit&amp;dapibus=amet&amp;augue=eros&amp;vel=suspendisse&amp;accumsan=accumsan&amp;tellus=tortor&amp;nisi=quis&amp;eu=turpis&amp;orci=sed&amp;mauris=ante&amp;lacinia=vivamus&amp;sapien=tortor&amp;quis=duis&amp;libero=mattis&amp;nullam=egestas&amp;sit=metus&amp;amet=aenean&amp;turpis=fermentum&amp;elementum=donec&amp;ligula=ut&amp;vehicula=mauris&amp;consequat=eget&amp;morbi=massa&amp;a=tempor&amp;ipsum=convallis&amp;integer=nulla&amp;a=neque&amp;nibh=libero</t>
+  </si>
+  <si>
+    <t>http://vistaprint.com/est/congue/elementum/in/hac.js?lacus=aliquet&amp;curabitur=massa&amp;at=id&amp;ipsum=lobortis&amp;ac=convallis</t>
+  </si>
+  <si>
+    <t>http://shutterfly.com/tempus/sit/amet.aspx?ac=non&amp;neque=mauris&amp;duis=morbi&amp;bibendum=non&amp;morbi=lectus&amp;non=aliquam&amp;quam=sit&amp;nec=amet&amp;dui=diam&amp;luctus=in&amp;rutrum=magna&amp;nulla=bibendum&amp;tellus=imperdiet&amp;in=nullam&amp;sagittis=orci</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/molestie/nibh/in/lectus/pellentesque.png?praesent=in&amp;lectus=hac&amp;vestibulum=habitasse&amp;quam=platea&amp;sapien=dictumst&amp;varius=morbi&amp;ut=vestibulum&amp;blandit=velit&amp;non=id&amp;interdum=pretium&amp;in=iaculis&amp;ante=diam&amp;vestibulum=erat&amp;ante=fermentum&amp;ipsum=justo&amp;primis=nec&amp;in=condimentum&amp;faucibus=neque&amp;orci=sapien&amp;luctus=placerat&amp;et=ante&amp;ultrices=nulla&amp;posuere=justo&amp;cubilia=aliquam&amp;curae=quis&amp;duis=turpis&amp;faucibus=eget&amp;accumsan=elit&amp;odio=sodales&amp;curabitur=scelerisque&amp;convallis=mauris&amp;duis=sit&amp;consequat=amet&amp;dui=eros&amp;nec=suspendisse&amp;nisi=accumsan&amp;volutpat=tortor&amp;eleifend=quis&amp;donec=turpis&amp;ut=sed&amp;dolor=ante&amp;morbi=vivamus&amp;vel=tortor&amp;lectus=duis&amp;in=mattis&amp;quam=egestas&amp;fringilla=metus&amp;rhoncus=aenean&amp;mauris=fermentum&amp;enim=donec&amp;leo=ut&amp;rhoncus=mauris</t>
+  </si>
+  <si>
+    <t>https://paypal.com/ligula/vehicula/consequat/morbi/a/ipsum.jsp?ipsum=justo&amp;integer=pellentesque&amp;a=viverra&amp;nibh=pede&amp;in=ac&amp;quis=diam&amp;justo=cras&amp;maecenas=pellentesque&amp;rhoncus=volutpat&amp;aliquam=dui&amp;lacus=maecenas&amp;morbi=tristique&amp;quis=est&amp;tortor=et&amp;id=tempus&amp;nulla=semper&amp;ultrices=est&amp;aliquet=quam&amp;maecenas=pharetra&amp;leo=magna&amp;odio=ac&amp;condimentum=consequat&amp;id=metus&amp;luctus=sapien&amp;nec=ut&amp;molestie=nunc&amp;sed=vestibulum&amp;justo=ante&amp;pellentesque=ipsum&amp;viverra=primis&amp;pede=in&amp;ac=faucibus&amp;diam=orci&amp;cras=luctus&amp;pellentesque=et&amp;volutpat=ultrices&amp;dui=posuere&amp;maecenas=cubilia&amp;tristique=curae&amp;est=mauris&amp;et=viverra&amp;tempus=diam&amp;semper=vitae&amp;est=quam&amp;quam=suspendisse&amp;pharetra=potenti&amp;magna=nullam&amp;ac=porttitor&amp;consequat=lacus&amp;metus=at&amp;sapien=turpis&amp;ut=donec&amp;nunc=posuere&amp;vestibulum=metus&amp;ante=vitae&amp;ipsum=ipsum&amp;primis=aliquam&amp;in=non&amp;faucibus=mauris&amp;orci=morbi&amp;luctus=non&amp;et=lectus&amp;ultrices=aliquam&amp;posuere=sit&amp;cubilia=amet&amp;curae=diam&amp;mauris=in&amp;viverra=magna&amp;diam=bibendum&amp;vitae=imperdiet&amp;quam=nullam&amp;suspendisse=orci&amp;potenti=pede&amp;nullam=venenatis&amp;porttitor=non&amp;lacus=sodales&amp;at=sed&amp;turpis=tincidunt&amp;donec=eu&amp;posuere=felis&amp;metus=fusce&amp;vitae=posuere&amp;ipsum=felis&amp;aliquam=sed&amp;non=lacus&amp;mauris=morbi&amp;morbi=sem&amp;non=mauris&amp;lectus=laoreet&amp;aliquam=ut</t>
+  </si>
+  <si>
+    <t>https://pcworld.com/in.json?suspendisse=arcu&amp;accumsan=sed&amp;tortor=augue&amp;quis=aliquam&amp;turpis=erat&amp;sed=volutpat&amp;ante=in&amp;vivamus=congue&amp;tortor=etiam&amp;duis=justo&amp;mattis=etiam&amp;egestas=pretium&amp;metus=iaculis&amp;aenean=justo&amp;fermentum=in&amp;donec=hac&amp;ut=habitasse&amp;mauris=platea&amp;eget=dictumst&amp;massa=etiam&amp;tempor=faucibus&amp;convallis=cursus&amp;nulla=urna&amp;neque=ut&amp;libero=tellus&amp;convallis=nulla&amp;eget=ut&amp;eleifend=erat&amp;luctus=id&amp;ultricies=mauris&amp;eu=vulputate&amp;nibh=elementum&amp;quisque=nullam&amp;id=varius&amp;justo=nulla&amp;sit=facilisi&amp;amet=cras&amp;sapien=non&amp;dignissim=velit&amp;vestibulum=nec&amp;vestibulum=nisi&amp;ante=vulputate&amp;ipsum=nonummy&amp;primis=maecenas&amp;in=tincidunt&amp;faucibus=lacus&amp;orci=at&amp;luctus=velit&amp;et=vivamus&amp;ultrices=vel&amp;posuere=nulla&amp;cubilia=eget&amp;curae=eros&amp;nulla=elementum&amp;dapibus=pellentesque&amp;dolor=quisque&amp;vel=porta&amp;est=volutpat&amp;donec=erat&amp;odio=quisque&amp;justo=erat&amp;sollicitudin=eros&amp;ut=viverra&amp;suscipit=eget&amp;a=congue&amp;feugiat=eget&amp;et=semper&amp;eros=rutrum&amp;vestibulum=nulla&amp;ac=nunc&amp;est=purus&amp;lacinia=phasellus&amp;nisi=in&amp;venenatis=felis&amp;tristique=donec</t>
+  </si>
+  <si>
+    <t>http://ted.com/ullamcorper/augue/a/suscipit.js?nulla=ipsum&amp;ac=integer&amp;enim=a&amp;in=nibh&amp;tempor=in&amp;turpis=quis&amp;nec=justo&amp;euismod=maecenas&amp;scelerisque=rhoncus&amp;quam=aliquam&amp;turpis=lacus&amp;adipiscing=morbi&amp;lorem=quis&amp;vitae=tortor&amp;mattis=id&amp;nibh=nulla&amp;ligula=ultrices&amp;nec=aliquet&amp;sem=maecenas&amp;duis=leo&amp;aliquam=odio&amp;convallis=condimentum&amp;nunc=id&amp;proin=luctus&amp;at=nec&amp;turpis=molestie&amp;a=sed&amp;pede=justo&amp;posuere=pellentesque&amp;nonummy=viverra&amp;integer=pede&amp;non=ac&amp;velit=diam</t>
+  </si>
+  <si>
+    <t>https://tumblr.com/consequat/nulla/nisl/nunc.json?ut=dictumst&amp;dolor=morbi&amp;morbi=vestibulum&amp;vel=velit&amp;lectus=id&amp;in=pretium&amp;quam=iaculis&amp;fringilla=diam&amp;rhoncus=erat&amp;mauris=fermentum&amp;enim=justo&amp;leo=nec&amp;rhoncus=condimentum&amp;sed=neque&amp;vestibulum=sapien&amp;sit=placerat&amp;amet=ante&amp;cursus=nulla&amp;id=justo&amp;turpis=aliquam&amp;integer=quis&amp;aliquet=turpis&amp;massa=eget&amp;id=elit&amp;lobortis=sodales&amp;convallis=scelerisque&amp;tortor=mauris&amp;risus=sit&amp;dapibus=amet&amp;augue=eros&amp;vel=suspendisse&amp;accumsan=accumsan&amp;tellus=tortor&amp;nisi=quis&amp;eu=turpis&amp;orci=sed&amp;mauris=ante</t>
+  </si>
+  <si>
+    <t>https://artisteer.com/accumsan/odio/curabitur/convallis/duis.jsp?cubilia=quis&amp;curae=orci&amp;donec=eget&amp;pharetra=orci&amp;magna=vehicula&amp;vestibulum=condimentum&amp;aliquet=curabitur&amp;ultrices=in&amp;erat=libero&amp;tortor=ut&amp;sollicitudin=massa&amp;mi=volutpat&amp;sit=convallis&amp;amet=morbi&amp;lobortis=odio&amp;sapien=odio&amp;sapien=elementum&amp;non=eu&amp;mi=interdum&amp;integer=eu&amp;ac=tincidunt&amp;neque=in</t>
+  </si>
+  <si>
+    <t>http://yale.edu/turpis/adipiscing.json?odio=dictumst&amp;curabitur=maecenas&amp;convallis=ut&amp;duis=massa&amp;consequat=quis&amp;dui=augue&amp;nec=luctus&amp;nisi=tincidunt&amp;volutpat=nulla&amp;eleifend=mollis&amp;donec=molestie&amp;ut=lorem&amp;dolor=quisque&amp;morbi=ut&amp;vel=erat&amp;lectus=curabitur&amp;in=gravida&amp;quam=nisi&amp;fringilla=at&amp;rhoncus=nibh&amp;mauris=in&amp;enim=hac&amp;leo=habitasse&amp;rhoncus=platea&amp;sed=dictumst&amp;vestibulum=aliquam&amp;sit=augue&amp;amet=quam&amp;cursus=sollicitudin&amp;id=vitae&amp;turpis=consectetuer&amp;integer=eget&amp;aliquet=rutrum&amp;massa=at&amp;id=lorem&amp;lobortis=integer&amp;convallis=tincidunt&amp;tortor=ante&amp;risus=vel&amp;dapibus=ipsum&amp;augue=praesent&amp;vel=blandit&amp;accumsan=lacinia&amp;tellus=erat&amp;nisi=vestibulum&amp;eu=sed&amp;orci=magna&amp;mauris=at&amp;lacinia=nunc&amp;sapien=commodo&amp;quis=placerat&amp;libero=praesent&amp;nullam=blandit&amp;sit=nam&amp;amet=nulla&amp;turpis=integer&amp;elementum=pede&amp;ligula=justo&amp;vehicula=lacinia&amp;consequat=eget&amp;morbi=tincidunt&amp;a=eget&amp;ipsum=tempus&amp;integer=vel&amp;a=pede&amp;nibh=morbi&amp;in=porttitor</t>
+  </si>
+  <si>
+    <t>http://weibo.com/ultrices/phasellus/id/sapien/in/sapien/iaculis.json?habitasse=aliquet&amp;platea=ultrices&amp;dictumst=erat&amp;aliquam=tortor&amp;augue=sollicitudin&amp;quam=mi&amp;sollicitudin=sit&amp;vitae=amet&amp;consectetuer=lobortis&amp;eget=sapien&amp;rutrum=sapien&amp;at=non&amp;lorem=mi&amp;integer=integer&amp;tincidunt=ac&amp;ante=neque&amp;vel=duis&amp;ipsum=bibendum&amp;praesent=morbi&amp;blandit=non&amp;lacinia=quam&amp;erat=nec&amp;vestibulum=dui&amp;sed=luctus&amp;magna=rutrum&amp;at=nulla&amp;nunc=tellus&amp;commodo=in&amp;placerat=sagittis&amp;praesent=dui&amp;blandit=vel&amp;nam=nisl&amp;nulla=duis&amp;integer=ac&amp;pede=nibh&amp;justo=fusce&amp;lacinia=lacus&amp;eget=purus&amp;tincidunt=aliquet&amp;eget=at&amp;tempus=feugiat&amp;vel=non&amp;pede=pretium&amp;morbi=quis&amp;porttitor=lectus&amp;lorem=suspendisse&amp;id=potenti</t>
+  </si>
+  <si>
+    <t>https://newyorker.com/in/porttitor/pede/justo/eu/massa/donec.aspx?quisque=ipsum&amp;erat=primis&amp;eros=in&amp;viverra=faucibus&amp;eget=orci&amp;congue=luctus&amp;eget=et&amp;semper=ultrices&amp;rutrum=posuere&amp;nulla=cubilia&amp;nunc=curae&amp;purus=mauris&amp;phasellus=viverra&amp;in=diam&amp;felis=vitae&amp;donec=quam&amp;semper=suspendisse&amp;sapien=potenti&amp;a=nullam&amp;libero=porttitor&amp;nam=lacus&amp;dui=at&amp;proin=turpis&amp;leo=donec&amp;odio=posuere&amp;porttitor=metus&amp;id=vitae&amp;consequat=ipsum&amp;in=aliquam&amp;consequat=non&amp;ut=mauris&amp;nulla=morbi&amp;sed=non&amp;accumsan=lectus&amp;felis=aliquam&amp;ut=sit&amp;at=amet&amp;dolor=diam</t>
+  </si>
+  <si>
+    <t>http://a8.net/libero/rutrum/ac/lobortis/vel/dapibus/at.jsp?in=orci&amp;hac=eget&amp;habitasse=orci&amp;platea=vehicula&amp;dictumst=condimentum&amp;etiam=curabitur&amp;faucibus=in&amp;cursus=libero&amp;urna=ut&amp;ut=massa&amp;tellus=volutpat&amp;nulla=convallis&amp;ut=morbi&amp;erat=odio&amp;id=odio&amp;mauris=elementum&amp;vulputate=eu&amp;elementum=interdum&amp;nullam=eu&amp;varius=tincidunt&amp;nulla=in&amp;facilisi=leo&amp;cras=maecenas&amp;non=pulvinar&amp;velit=lobortis&amp;nec=est&amp;nisi=phasellus&amp;vulputate=sit&amp;nonummy=amet&amp;maecenas=erat&amp;tincidunt=nulla&amp;lacus=tempus&amp;at=vivamus&amp;velit=in&amp;vivamus=felis&amp;vel=eu&amp;nulla=sapien&amp;eget=cursus&amp;eros=vestibulum&amp;elementum=proin&amp;pellentesque=eu&amp;quisque=mi&amp;porta=nulla&amp;volutpat=ac&amp;erat=enim&amp;quisque=in&amp;erat=tempor&amp;eros=turpis&amp;viverra=nec&amp;eget=euismod&amp;congue=scelerisque&amp;eget=quam&amp;semper=turpis&amp;rutrum=adipiscing&amp;nulla=lorem&amp;nunc=vitae&amp;purus=mattis&amp;phasellus=nibh&amp;in=ligula&amp;felis=nec&amp;donec=sem&amp;semper=duis&amp;sapien=aliquam&amp;a=convallis&amp;libero=nunc&amp;nam=proin&amp;dui=at&amp;proin=turpis&amp;leo=a&amp;odio=pede&amp;porttitor=posuere&amp;id=nonummy&amp;consequat=integer&amp;in=non&amp;consequat=velit&amp;ut=donec&amp;nulla=diam&amp;sed=neque&amp;accumsan=vestibulum&amp;felis=eget</t>
+  </si>
+  <si>
+    <t>http://comcast.net/volutpat.json?semper=nulla&amp;est=tellus&amp;quam=in&amp;pharetra=sagittis&amp;magna=dui&amp;ac=vel&amp;consequat=nisl&amp;metus=duis&amp;sapien=ac&amp;ut=nibh&amp;nunc=fusce&amp;vestibulum=lacus&amp;ante=purus&amp;ipsum=aliquet&amp;primis=at&amp;in=feugiat&amp;faucibus=non&amp;orci=pretium&amp;luctus=quis&amp;et=lectus&amp;ultrices=suspendisse&amp;posuere=potenti&amp;cubilia=in&amp;curae=eleifend&amp;mauris=quam&amp;viverra=a&amp;diam=odio&amp;vitae=in&amp;quam=hac&amp;suspendisse=habitasse&amp;potenti=platea&amp;nullam=dictumst&amp;porttitor=maecenas&amp;lacus=ut&amp;at=massa&amp;turpis=quis&amp;donec=augue&amp;posuere=luctus&amp;metus=tincidunt&amp;vitae=nulla&amp;ipsum=mollis&amp;aliquam=molestie&amp;non=lorem&amp;mauris=quisque&amp;morbi=ut&amp;non=erat&amp;lectus=curabitur&amp;aliquam=gravida&amp;sit=nisi&amp;amet=at&amp;diam=nibh&amp;in=in&amp;magna=hac&amp;bibendum=habitasse&amp;imperdiet=platea&amp;nullam=dictumst&amp;orci=aliquam&amp;pede=augue&amp;venenatis=quam&amp;non=sollicitudin&amp;sodales=vitae&amp;sed=consectetuer&amp;tincidunt=eget&amp;eu=rutrum&amp;felis=at&amp;fusce=lorem&amp;posuere=integer&amp;felis=tincidunt&amp;sed=ante&amp;lacus=vel&amp;morbi=ipsum&amp;sem=praesent&amp;mauris=blandit&amp;laoreet=lacinia&amp;ut=erat&amp;rhoncus=vestibulum&amp;aliquet=sed&amp;pulvinar=magna&amp;sed=at&amp;nisl=nunc&amp;nunc=commodo&amp;rhoncus=placerat&amp;dui=praesent&amp;vel=blandit&amp;sem=nam&amp;sed=nulla&amp;sagittis=integer&amp;nam=pede&amp;congue=justo&amp;risus=lacinia&amp;semper=eget&amp;porta=tincidunt&amp;volutpat=eget</t>
+  </si>
+  <si>
+    <t>https://vk.com/blandit/nam/nulla/integer/pede.html?pede=ridiculus&amp;morbi=mus&amp;porttitor=vivamus&amp;lorem=vestibulum&amp;id=sagittis&amp;ligula=sapien&amp;suspendisse=cum&amp;ornare=sociis&amp;consequat=natoque&amp;lectus=penatibus&amp;in=et&amp;est=magnis&amp;risus=dis&amp;auctor=parturient&amp;sed=montes&amp;tristique=nascetur&amp;in=ridiculus&amp;tempus=mus&amp;sit=etiam&amp;amet=vel&amp;sem=augue&amp;fusce=vestibulum&amp;consequat=rutrum&amp;nulla=rutrum&amp;nisl=neque&amp;nunc=aenean&amp;nisl=auctor&amp;duis=gravida&amp;bibendum=sem&amp;felis=praesent&amp;sed=id&amp;interdum=massa&amp;venenatis=id&amp;turpis=nisl&amp;enim=venenatis&amp;blandit=lacinia&amp;mi=aenean&amp;in=sit&amp;porttitor=amet&amp;pede=justo&amp;justo=morbi&amp;eu=ut&amp;massa=odio&amp;donec=cras&amp;dapibus=mi&amp;duis=pede&amp;at=malesuada&amp;velit=in&amp;eu=imperdiet&amp;est=et&amp;congue=commodo&amp;elementum=vulputate&amp;in=justo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -1188,11 +1251,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1270,7 @@
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1232,8 +1295,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1258,8 +1324,11 @@
       <c r="H2" s="1">
         <v>57978.09</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1284,8 +1353,11 @@
       <c r="H3" s="1">
         <v>41761.279999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1310,8 +1382,11 @@
       <c r="H4" s="1">
         <v>45132.18</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1336,8 +1411,11 @@
       <c r="H5" s="1">
         <v>67266.289999999994</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1362,8 +1440,11 @@
       <c r="H6" s="1">
         <v>53925.74</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1388,8 +1469,11 @@
       <c r="H7" s="1">
         <v>54523.77</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1414,8 +1498,11 @@
       <c r="H8" s="1">
         <v>42758.48</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1440,8 +1527,11 @@
       <c r="H9" s="1">
         <v>41256.78</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1466,8 +1556,11 @@
       <c r="H10" s="1">
         <v>62117.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1492,8 +1585,11 @@
       <c r="H11" s="1">
         <v>63298.27</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1518,8 +1614,11 @@
       <c r="H12" s="1">
         <v>51552.07</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1544,8 +1643,11 @@
       <c r="H13" s="1">
         <v>49906.43</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1570,8 +1672,11 @@
       <c r="H14" s="1">
         <v>50252.91</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1596,8 +1701,11 @@
       <c r="H15" s="1">
         <v>51160.93</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1622,8 +1730,11 @@
       <c r="H16" s="1">
         <v>61115.37</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1648,8 +1759,11 @@
       <c r="H17" s="1">
         <v>69050.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1674,8 +1788,11 @@
       <c r="H18" s="1">
         <v>48265.66</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1700,8 +1817,11 @@
       <c r="H19" s="1">
         <v>62952.41</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1726,8 +1846,11 @@
       <c r="H20" s="1">
         <v>40706.22</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1751,6 +1874,9 @@
       </c>
       <c r="H21" s="1">
         <v>68271.62</v>
+      </c>
+      <c r="I21" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>